<commit_message>
aggiunta parte bn e kb
</commit_message>
<xml_diff>
--- a/agent/pgm/bif/charts.xlsx
+++ b/agent/pgm/bif/charts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\icon-745751\agent\pgm\bif\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="query1-3" sheetId="4" r:id="rId1"/>
     <sheet name="query4-11" sheetId="1" r:id="rId2"/>
-    <sheet name="query12-13" sheetId="2" r:id="rId3"/>
+    <sheet name="query12" sheetId="2" r:id="rId3"/>
+    <sheet name="query13" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
   <si>
     <t>page_template</t>
   </si>
@@ -35,12 +36,6 @@
   </si>
   <si>
     <t>MAP</t>
-  </si>
-  <si>
-    <t>P(page_template | page_ungrouped_multim=1)</t>
-  </si>
-  <si>
-    <t>P(page_template | page_ungrouped_multim=3)</t>
   </si>
   <si>
     <t>P(page_template | NDOM_nodes=1, NDOM_height=1, metric=4)</t>
@@ -91,7 +86,37 @@
     <t>4 [4, 5]</t>
   </si>
   <si>
-    <t>P(page_template | page_ungrouped_multim=4)</t>
+    <t>P(NDOM_nodes, NDOM_height | page_template=1)</t>
+  </si>
+  <si>
+    <t>NDOM_nodes</t>
+  </si>
+  <si>
+    <t>NDOM_height</t>
+  </si>
+  <si>
+    <t>1 [0, 500]</t>
+  </si>
+  <si>
+    <t>1 [0, 4]</t>
+  </si>
+  <si>
+    <t>2 [5-13]</t>
+  </si>
+  <si>
+    <t>3 [14+]</t>
+  </si>
+  <si>
+    <t>2 [501, 1000]</t>
+  </si>
+  <si>
+    <t>3 [1001, 1500]</t>
+  </si>
+  <si>
+    <t>4 [1501+]</t>
+  </si>
+  <si>
+    <t>P(page_template | page_ungrouped_multim=3)</t>
   </si>
 </sst>
 </file>
@@ -133,8 +158,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -886,7 +912,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -987,7 +1012,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1117,7 +1141,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1314,7 +1337,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1424,7 +1446,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1525,7 +1546,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1655,7 +1675,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1852,7 +1871,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1934,6 +1952,34 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050">
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>P(NDOM_nodes, NDOM_height | page_template=1)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1972,113 +2018,18 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'query12-13'!$B$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MLE</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'query12-13'!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'query12-13'!$B$3:$B$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.5399999999999998E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.2000000000000007E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.44E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.10680000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.58109999999999995</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.3400000000000003E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.10059999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0100000000000005E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5472-4C1F-8ACB-2094011DEA97}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'query12-13'!$C$2</c:f>
+              <c:f>query12!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>MAP</c:v>
                 </c:pt>
               </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:strRef>
           </c:tx>
           <c:spPr>
@@ -2091,81 +2042,206 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>'query12-13'!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>query12!$A$3:$B$14</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1 [0, 4]</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2 [5-13]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3 [14+]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1 [0, 4]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2 [5-13]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3 [14+]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1 [0, 4]</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2 [5-13]</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3 [14+]</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1 [0, 4]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2 [5-13]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3 [14+]</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1 [0, 500]</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1 [0, 500]</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1 [0, 500]</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2 [501, 1000]</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2 [501, 1000]</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2 [501, 1000]</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3 [1001, 1500]</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3 [1001, 1500]</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>3 [1001, 1500]</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>4 [1501+]</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>4 [1501+]</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>4 [1501+]</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'query12-13'!$C$3:$C$11</c:f>
+              <c:f>query12!$D$3:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5.4899999999999997E-2</c:v>
+                  <c:v>5.7099999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.06E-2</c:v>
+                  <c:v>0.71870000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.44E-2</c:v>
+                  <c:v>1.47E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1003</c:v>
+                  <c:v>6.8999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57820000000000005</c:v>
+                  <c:v>0.1116</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.6000000000000001E-2</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10589999999999999</c:v>
+                  <c:v>2.7000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.9600000000000004E-2</c:v>
+                  <c:v>4.1200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.2000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.7100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0999999999999999E-3</c:v>
                 </c:pt>
               </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5472-4C1F-8ACB-2094011DEA97}"/>
+              <c16:uniqueId val="{00000001-9E66-41C4-8A9B-ADA12191268B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2173,11 +2249,253 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1131278095"/>
-        <c:axId val="1131283503"/>
+        <c:axId val="1102209055"/>
+        <c:axId val="1102204063"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>query12!$C$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>MLE</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="it-IT"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:layout/>
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>query12!$A$3:$B$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="12"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>1 [0, 4]</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>2 [5-13]</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>3 [14+]</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>1 [0, 4]</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>2 [5-13]</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>3 [14+]</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>1 [0, 4]</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>2 [5-13]</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>3 [14+]</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>1 [0, 4]</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>2 [5-13]</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>3 [14+]</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>1 [0, 500]</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>1 [0, 500]</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>1 [0, 500]</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
+                          <c:v>2 [501, 1000]</c:v>
+                        </c:pt>
+                        <c:pt idx="4">
+                          <c:v>2 [501, 1000]</c:v>
+                        </c:pt>
+                        <c:pt idx="5">
+                          <c:v>2 [501, 1000]</c:v>
+                        </c:pt>
+                        <c:pt idx="6">
+                          <c:v>3 [1001, 1500]</c:v>
+                        </c:pt>
+                        <c:pt idx="7">
+                          <c:v>3 [1001, 1500]</c:v>
+                        </c:pt>
+                        <c:pt idx="8">
+                          <c:v>3 [1001, 1500]</c:v>
+                        </c:pt>
+                        <c:pt idx="9">
+                          <c:v>4 [1501+]</c:v>
+                        </c:pt>
+                        <c:pt idx="10">
+                          <c:v>4 [1501+]</c:v>
+                        </c:pt>
+                        <c:pt idx="11">
+                          <c:v>4 [1501+]</c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>query12!$C$3:$C$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>1.4999999999999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.86350000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>8.0000000000000004E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.11</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.8999999999999998E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>6.7999999999999996E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-9E66-41C4-8A9B-ADA12191268B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1131278095"/>
+        <c:axId val="1102209055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2220,7 +2538,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1131283503"/>
+        <c:crossAx val="1102204063"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2228,10 +2546,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1131283503"/>
+        <c:axId val="1102204063"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2280,7 +2597,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1131278095"/>
+        <c:crossAx val="1102209055"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2292,38 +2609,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2376,7 +2661,34 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050">
+                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>P(page_template | page_ungrouped_multim=3)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2414,107 +2726,11 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'query12-13'!$D$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MLE</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'query12-13'!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'query12-13'!$D$3:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>3.4700000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.6300000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.79E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.8600000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.1158</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.09E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.64859999999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-41EB-409C-8D8E-8778551B5FB6}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'query12-13'!$E$2</c:f>
+              <c:f>query13!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2533,12 +2749,70 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'query12-13'!$A$3:$A$11</c:f>
+              <c:f>query13!$A$3:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2568,10 +2842,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'query12-13'!$E$3:$E$11</c:f>
+              <c:f>query13!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>3.2800000000000003E-2</c:v>
                 </c:pt>
@@ -2601,13 +2875,14 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-41EB-409C-8D8E-8778551B5FB6}"/>
+              <c16:uniqueId val="{00000001-F825-44B4-87B2-5CFCA0AA1384}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2615,11 +2890,189 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1131278095"/>
-        <c:axId val="1131283503"/>
+        <c:axId val="1895921088"/>
+        <c:axId val="1895919008"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>query13!$B$2</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>MLE</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="it-IT"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>query13!$A$3:$A$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>5</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>7</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>8</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>query13!$B$3:$B$10</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="8"/>
+                      <c:pt idx="0">
+                        <c:v>3.4700000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>4.6300000000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.7E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5.79E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>3.8600000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.1158</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>3.09E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.64859999999999995</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-F825-44B4-87B2-5CFCA0AA1384}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1131278095"/>
+        <c:axId val="1895921088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2662,7 +3115,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1131283503"/>
+        <c:crossAx val="1895919008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2670,7 +3123,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1131283503"/>
+        <c:axId val="1895919008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2722,9 +3175,10 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1131278095"/>
+        <c:crossAx val="1895921088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2734,480 +3188,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'query12-13'!$F$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MLE</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'query12-13'!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'query12-13'!$F$3:$F$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.8099999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.9800000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.1599999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.8099999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.1047</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.14E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.61629999999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7410-477E-BEA8-D06086675EEC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'query12-13'!$G$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MAP</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'query12-13'!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'query12-13'!$G$3:$G$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>5.0099999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0099999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0700000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.9299999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.03E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.9299999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.51E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.62509999999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7410-477E-BEA8-D06086675EEC}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1131278095"/>
-        <c:axId val="1131283503"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1131278095"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1131283503"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1131283503"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1131278095"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4603,7 +4583,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4704,7 +4683,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4834,7 +4812,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5031,7 +5008,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5141,7 +5117,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5242,7 +5217,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5372,7 +5346,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5569,7 +5542,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5679,7 +5651,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5780,7 +5751,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5910,7 +5880,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6107,7 +6076,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6217,7 +6185,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6318,7 +6285,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6448,7 +6414,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6645,7 +6610,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6755,7 +6719,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6856,7 +6819,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6986,7 +6948,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7183,7 +7144,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7293,7 +7253,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7394,7 +7353,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7524,7 +7482,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -7721,7 +7678,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7949,46 +7905,6 @@
 </file>
 
 <file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10361,509 +10277,6 @@
 </file>
 
 <file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15752,20 +15165,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>995362</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Grafico 2"/>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -15780,25 +15193,28 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1476375</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Grafico 4"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Grafico 2"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -15806,39 +15222,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1533525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Grafico 5"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -16112,7 +15496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
@@ -16128,18 +15512,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -16364,7 +15748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView topLeftCell="H25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -16387,42 +15771,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -16475,7 +15859,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -16528,7 +15912,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>5.1900000000000002E-2</v>
@@ -16581,7 +15965,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0.42009999999999997</v>
@@ -16634,7 +16018,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>0.52810000000000001</v>
@@ -16703,39 +16087,247 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D3">
+        <v>5.7099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>0.86350000000000005</v>
+      </c>
+      <c r="D4">
+        <v>0.71870000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1.47E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D6">
+        <v>6.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>0.11</v>
+      </c>
+      <c r="D7">
+        <v>0.1116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="D10">
+        <v>4.1200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1.6999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2.2000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="D13">
+        <v>3.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2.0999999999999999E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -16744,208 +16336,98 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.5399999999999998E-2</v>
+        <v>3.4700000000000002E-2</v>
       </c>
       <c r="C3">
-        <v>5.4899999999999997E-2</v>
-      </c>
-      <c r="D3">
-        <v>3.4700000000000002E-2</v>
-      </c>
-      <c r="E3">
         <v>3.2800000000000003E-2</v>
       </c>
-      <c r="F3">
-        <v>5.8099999999999999E-2</v>
-      </c>
-      <c r="G3">
-        <v>5.0099999999999999E-2</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>8.2000000000000007E-3</v>
+        <v>4.6300000000000001E-2</v>
       </c>
       <c r="C4">
-        <v>1.06E-2</v>
-      </c>
-      <c r="D4">
-        <v>4.6300000000000001E-2</v>
-      </c>
-      <c r="E4">
         <v>4.4699999999999997E-2</v>
       </c>
-      <c r="F4">
-        <v>6.9800000000000001E-2</v>
-      </c>
-      <c r="G4">
-        <v>5.0099999999999999E-2</v>
-      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.44E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="C5">
-        <v>1.44E-2</v>
-      </c>
-      <c r="D5">
-        <v>2.7E-2</v>
-      </c>
-      <c r="E5">
         <v>1.6400000000000001E-2</v>
       </c>
-      <c r="F5">
-        <v>1.1599999999999999E-2</v>
-      </c>
-      <c r="G5">
-        <v>3.0700000000000002E-2</v>
-      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.10680000000000001</v>
+        <v>5.79E-2</v>
       </c>
       <c r="C6">
-        <v>0.1003</v>
-      </c>
-      <c r="D6">
-        <v>5.79E-2</v>
-      </c>
-      <c r="E6">
         <v>5.74E-2</v>
       </c>
-      <c r="F6">
-        <v>5.8099999999999999E-2</v>
-      </c>
-      <c r="G6">
-        <v>5.9299999999999999E-2</v>
-      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.58109999999999995</v>
+        <v>3.8600000000000002E-2</v>
       </c>
       <c r="C7">
-        <v>0.57820000000000005</v>
-      </c>
-      <c r="D7">
-        <v>3.8600000000000002E-2</v>
-      </c>
-      <c r="E7">
         <v>4.0399999999999998E-2</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>1.03E-2</v>
-      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5.3400000000000003E-2</v>
+        <v>0.1158</v>
       </c>
       <c r="C8">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="D8">
-        <v>0.1158</v>
-      </c>
-      <c r="E8">
         <v>0.11269999999999999</v>
       </c>
-      <c r="F8">
-        <v>0.1047</v>
-      </c>
-      <c r="G8">
-        <v>9.9299999999999999E-2</v>
-      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.10059999999999999</v>
+        <v>3.09E-2</v>
       </c>
       <c r="C9">
-        <v>0.10589999999999999</v>
-      </c>
-      <c r="D9">
-        <v>3.09E-2</v>
-      </c>
-      <c r="E9">
         <v>3.3500000000000002E-2</v>
       </c>
-      <c r="F9">
-        <v>8.14E-2</v>
-      </c>
-      <c r="G9">
-        <v>7.51E-2</v>
-      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8.0100000000000005E-2</v>
+        <v>0.64859999999999995</v>
       </c>
       <c r="C10">
-        <v>7.9600000000000004E-2</v>
-      </c>
-      <c r="D10">
-        <v>0.64859999999999995</v>
-      </c>
-      <c r="E10">
         <v>0.66200000000000003</v>
-      </c>
-      <c r="F10">
-        <v>0.61629999999999996</v>
-      </c>
-      <c r="G10">
-        <v>0.62509999999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>